<commit_message>
release finale -> funzionante e testato
</commit_message>
<xml_diff>
--- a/template_excel/template_PEMS_HH.xlsx
+++ b/template_excel/template_PEMS_HH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhoaenergy.sharepoint.com/sites/Q1043-HyESScontainerHDevolution/Documenti condivisi/General/08_SW standardization/11_Alarms_Template/Alarms_automation_HH/template_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{211109C0-06BE-4724-B66C-088394B44761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB1758EB-A679-45C2-9A3E-3D804E3108E3}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{211109C0-06BE-4724-B66C-088394B44761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03C4C31D-A427-4181-AFD2-F26170D83F97}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CD33084-19B4-4D94-94A9-A50BCDD56A5B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CD33084-19B4-4D94-94A9-A50BCDD56A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,9 +407,6 @@
   </si>
   <si>
     <t>A | State Machine 2 in Alarm | PEMS</t>
-  </si>
-  <si>
-    <t>W | Spare</t>
   </si>
   <si>
     <t>W | battery room high average temperature | PEMS</t>
@@ -899,6 +896,9 @@
   <si>
     <t>_DiagnosticDB_wHMI_Warning5</t>
   </si>
+  <si>
+    <t>W | Spare wHMI_Warning3.9 | PEMS</t>
+  </si>
 </sst>
 </file>
 
@@ -952,7 +952,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -978,12 +978,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1281,36 +1277,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA43B29A-04EE-44AD-9859-14DB37742306}">
   <dimension ref="A1:AS160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D1" t="s">
         <v>44</v>
@@ -1439,15 +1435,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -1576,15 +1572,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -1713,15 +1709,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D4" t="s">
         <v>47</v>
@@ -1850,15 +1846,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1987,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1995,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D6" t="s">
         <v>49</v>
@@ -2124,15 +2120,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
@@ -2261,15 +2257,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
         <v>51</v>
@@ -2398,15 +2394,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D9" t="s">
         <v>52</v>
@@ -2535,15 +2531,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10" t="s">
         <v>53</v>
@@ -2672,15 +2668,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>
@@ -2809,15 +2805,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
         <v>222</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>223</v>
       </c>
       <c r="D12" t="s">
         <v>55</v>
@@ -2946,15 +2942,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
         <v>56</v>
@@ -3083,15 +3079,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
         <v>57</v>
@@ -3220,15 +3216,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
@@ -3357,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -3365,7 +3361,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D16" t="s">
         <v>59</v>
@@ -3494,15 +3490,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D17" t="s">
         <v>44</v>
@@ -3532,7 +3528,7 @@
         <v>42</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N17" t="s">
         <v>41</v>
@@ -3631,15 +3627,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D18" t="s">
         <v>45</v>
@@ -3768,15 +3764,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
@@ -3905,15 +3901,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D20" t="s">
         <v>47</v>
@@ -4042,15 +4038,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -4179,15 +4175,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D22" t="s">
         <v>49</v>
@@ -4316,15 +4312,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D23" t="s">
         <v>50</v>
@@ -4453,15 +4449,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -4590,15 +4586,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D25" t="s">
         <v>52</v>
@@ -4727,15 +4723,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D26" t="s">
         <v>53</v>
@@ -4864,15 +4860,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -5001,15 +4997,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D28" t="s">
         <v>55</v>
@@ -5138,15 +5134,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -5275,15 +5271,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D30" t="s">
         <v>57</v>
@@ -5412,15 +5408,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D31" t="s">
         <v>58</v>
@@ -5549,15 +5545,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D32" t="s">
         <v>59</v>
@@ -5686,15 +5682,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D33" t="s">
         <v>44</v>
@@ -5823,15 +5819,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D34" t="s">
         <v>45</v>
@@ -5960,15 +5956,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B35" t="s">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D35" t="s">
         <v>46</v>
@@ -6097,15 +6093,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D36" t="s">
         <v>47</v>
@@ -6234,15 +6230,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D37" t="s">
         <v>48</v>
@@ -6371,15 +6367,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s">
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D38" t="s">
         <v>49</v>
@@ -6508,15 +6504,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B39" t="s">
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D39" t="s">
         <v>50</v>
@@ -6645,15 +6641,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D40" t="s">
         <v>51</v>
@@ -6782,15 +6778,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -6919,15 +6915,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
@@ -7056,15 +7052,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
@@ -7193,15 +7189,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D44" t="s">
         <v>55</v>
@@ -7330,15 +7326,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D45" t="s">
         <v>56</v>
@@ -7467,15 +7463,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B46" t="s">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D46" t="s">
         <v>57</v>
@@ -7604,15 +7600,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D47" t="s">
         <v>58</v>
@@ -7741,15 +7737,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D48" t="s">
         <v>59</v>
@@ -7878,15 +7874,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B49" t="s">
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D49" t="s">
         <v>44</v>
@@ -8015,15 +8011,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D50" t="s">
         <v>45</v>
@@ -8152,15 +8148,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D51" t="s">
         <v>46</v>
@@ -8289,15 +8285,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D52" t="s">
         <v>47</v>
@@ -8426,15 +8422,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D53" t="s">
         <v>48</v>
@@ -8563,15 +8559,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B54" t="s">
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D54" t="s">
         <v>49</v>
@@ -8700,15 +8696,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B55" t="s">
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D55" t="s">
         <v>50</v>
@@ -8837,15 +8833,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B56" t="s">
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D56" t="s">
         <v>51</v>
@@ -8974,15 +8970,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B57" t="s">
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D57" t="s">
         <v>52</v>
@@ -9111,15 +9107,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B58" t="s">
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D58" t="s">
         <v>53</v>
@@ -9248,15 +9244,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D59" t="s">
         <v>54</v>
@@ -9385,15 +9381,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B60" t="s">
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D60" t="s">
         <v>55</v>
@@ -9522,15 +9518,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D61" t="s">
         <v>56</v>
@@ -9659,7 +9655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -9667,7 +9663,7 @@
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D62" t="s">
         <v>57</v>
@@ -9796,7 +9792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -9804,7 +9800,7 @@
         <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D63" t="s">
         <v>58</v>
@@ -9933,7 +9929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -9941,7 +9937,7 @@
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D64" t="s">
         <v>59</v>
@@ -10070,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -10078,7 +10074,7 @@
         <v>0</v>
       </c>
       <c r="C65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D65" t="s">
         <v>44</v>
@@ -10207,7 +10203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -10215,7 +10211,7 @@
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D66" t="s">
         <v>45</v>
@@ -10344,7 +10340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -10352,7 +10348,7 @@
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D67" t="s">
         <v>46</v>
@@ -10481,15 +10477,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B68" t="s">
         <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D68" t="s">
         <v>47</v>
@@ -10618,15 +10614,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
       </c>
       <c r="C69" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D69" t="s">
         <v>48</v>
@@ -10755,15 +10751,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B70" t="s">
         <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D70" t="s">
         <v>49</v>
@@ -10892,15 +10888,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B71" t="s">
         <v>0</v>
       </c>
       <c r="C71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D71" t="s">
         <v>50</v>
@@ -11029,7 +11025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -11037,7 +11033,7 @@
         <v>0</v>
       </c>
       <c r="C72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D72" t="s">
         <v>51</v>
@@ -11166,15 +11162,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B73" t="s">
         <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D73" t="s">
         <v>52</v>
@@ -11303,15 +11299,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B74" t="s">
         <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D74" t="s">
         <v>53</v>
@@ -11440,15 +11436,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D75" t="s">
         <v>54</v>
@@ -11577,15 +11573,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B76" t="s">
         <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D76" t="s">
         <v>55</v>
@@ -11714,15 +11710,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D77" t="s">
         <v>56</v>
@@ -11851,15 +11847,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D78" t="s">
         <v>57</v>
@@ -11988,7 +11984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>70</v>
       </c>
@@ -11996,7 +11992,7 @@
         <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D79" t="s">
         <v>58</v>
@@ -12125,7 +12121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>71</v>
       </c>
@@ -12133,7 +12129,7 @@
         <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D80" t="s">
         <v>59</v>
@@ -12262,15 +12258,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B81" t="s">
         <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D81" t="s">
         <v>44</v>
@@ -12399,15 +12395,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B82" t="s">
         <v>24</v>
       </c>
       <c r="C82" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D82" t="s">
         <v>45</v>
@@ -12536,15 +12532,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B83" t="s">
         <v>24</v>
       </c>
       <c r="C83" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D83" t="s">
         <v>46</v>
@@ -12673,15 +12669,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B84" t="s">
         <v>24</v>
       </c>
       <c r="C84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D84" t="s">
         <v>47</v>
@@ -12810,15 +12806,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B85" t="s">
         <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D85" t="s">
         <v>48</v>
@@ -12947,15 +12943,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B86" t="s">
         <v>24</v>
       </c>
       <c r="C86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D86" t="s">
         <v>49</v>
@@ -13084,15 +13080,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B87" t="s">
         <v>24</v>
       </c>
       <c r="C87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D87" t="s">
         <v>50</v>
@@ -13221,15 +13217,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B88" t="s">
         <v>24</v>
       </c>
       <c r="C88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D88" t="s">
         <v>51</v>
@@ -13358,15 +13354,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B89" t="s">
         <v>24</v>
       </c>
       <c r="C89" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D89" t="s">
         <v>52</v>
@@ -13495,15 +13491,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B90" t="s">
         <v>24</v>
       </c>
       <c r="C90" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D90" t="s">
         <v>53</v>
@@ -13632,15 +13628,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B91" t="s">
         <v>24</v>
       </c>
       <c r="C91" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D91" t="s">
         <v>54</v>
@@ -13769,15 +13765,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B92" t="s">
         <v>24</v>
       </c>
       <c r="C92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D92" t="s">
         <v>55</v>
@@ -13906,15 +13902,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B93" t="s">
         <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D93" t="s">
         <v>56</v>
@@ -14043,15 +14039,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B94" t="s">
         <v>24</v>
       </c>
       <c r="C94" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D94" t="s">
         <v>57</v>
@@ -14180,15 +14176,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B95" t="s">
         <v>24</v>
       </c>
       <c r="C95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D95" t="s">
         <v>58</v>
@@ -14317,15 +14313,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B96" t="s">
         <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D96" t="s">
         <v>59</v>
@@ -14454,15 +14450,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B97" t="s">
         <v>24</v>
       </c>
       <c r="C97" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D97" t="s">
         <v>44</v>
@@ -14591,15 +14587,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B98" t="s">
         <v>24</v>
       </c>
       <c r="C98" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D98" t="s">
         <v>45</v>
@@ -14728,15 +14724,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B99" t="s">
         <v>24</v>
       </c>
       <c r="C99" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D99" t="s">
         <v>46</v>
@@ -14865,15 +14861,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" t="s">
         <v>24</v>
       </c>
       <c r="C100" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D100" t="s">
         <v>47</v>
@@ -15002,15 +14998,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B101" t="s">
         <v>24</v>
       </c>
       <c r="C101" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D101" t="s">
         <v>48</v>
@@ -15139,15 +15135,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B102" t="s">
         <v>24</v>
       </c>
       <c r="C102" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D102" t="s">
         <v>49</v>
@@ -15276,15 +15272,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B103" t="s">
         <v>24</v>
       </c>
       <c r="C103" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D103" t="s">
         <v>50</v>
@@ -15413,15 +15409,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B104" t="s">
         <v>24</v>
       </c>
       <c r="C104" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D104" t="s">
         <v>51</v>
@@ -15550,15 +15546,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B105" t="s">
         <v>24</v>
       </c>
       <c r="C105" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D105" t="s">
         <v>52</v>
@@ -15687,15 +15683,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s">
         <v>24</v>
       </c>
       <c r="C106" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D106" t="s">
         <v>53</v>
@@ -15824,15 +15820,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B107" t="s">
         <v>24</v>
       </c>
       <c r="C107" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D107" t="s">
         <v>54</v>
@@ -15961,15 +15957,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B108" t="s">
         <v>24</v>
       </c>
       <c r="C108" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D108" t="s">
         <v>55</v>
@@ -16098,15 +16094,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
         <v>24</v>
       </c>
       <c r="C109" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D109" t="s">
         <v>56</v>
@@ -16235,15 +16231,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
         <v>24</v>
       </c>
       <c r="C110" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D110" t="s">
         <v>57</v>
@@ -16372,15 +16368,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B111" t="s">
         <v>24</v>
       </c>
       <c r="C111" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D111" t="s">
         <v>58</v>
@@ -16509,15 +16505,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B112" t="s">
         <v>24</v>
       </c>
       <c r="C112" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D112" t="s">
         <v>59</v>
@@ -16646,15 +16642,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B113" t="s">
         <v>24</v>
       </c>
       <c r="C113" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D113" t="s">
         <v>44</v>
@@ -16783,15 +16779,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B114" t="s">
         <v>24</v>
       </c>
       <c r="C114" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D114" t="s">
         <v>45</v>
@@ -16920,15 +16916,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B115" t="s">
         <v>24</v>
       </c>
       <c r="C115" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D115" t="s">
         <v>46</v>
@@ -17057,15 +17053,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B116" t="s">
         <v>24</v>
       </c>
       <c r="C116" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D116" t="s">
         <v>47</v>
@@ -17194,15 +17190,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B117" t="s">
         <v>24</v>
       </c>
       <c r="C117" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D117" t="s">
         <v>48</v>
@@ -17331,15 +17327,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B118" t="s">
         <v>24</v>
       </c>
       <c r="C118" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D118" t="s">
         <v>49</v>
@@ -17468,15 +17464,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B119" t="s">
         <v>24</v>
       </c>
       <c r="C119" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D119" t="s">
         <v>50</v>
@@ -17605,15 +17601,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B120" t="s">
         <v>24</v>
       </c>
       <c r="C120" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D120" t="s">
         <v>51</v>
@@ -17742,15 +17738,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B121" t="s">
         <v>24</v>
       </c>
       <c r="C121" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D121" t="s">
         <v>52</v>
@@ -17879,15 +17875,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>72</v>
+        <v>232</v>
       </c>
       <c r="B122" t="s">
         <v>24</v>
       </c>
       <c r="C122" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D122" t="s">
         <v>53</v>
@@ -18016,15 +18012,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:45" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:45" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B123" t="s">
         <v>24</v>
       </c>
       <c r="C123" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D123" t="s">
         <v>54</v>
@@ -18153,15 +18149,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:45" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:45" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B124" t="s">
         <v>24</v>
       </c>
       <c r="C124" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D124" s="3">
         <v>11</v>
@@ -18290,15 +18286,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B125" t="s">
         <v>24</v>
       </c>
       <c r="C125" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D125" t="s">
         <v>56</v>
@@ -18427,15 +18423,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B126" t="s">
         <v>24</v>
       </c>
       <c r="C126" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D126" t="s">
         <v>57</v>
@@ -18564,15 +18560,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B127" t="s">
         <v>24</v>
       </c>
       <c r="C127" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D127" t="s">
         <v>58</v>
@@ -18701,15 +18697,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B128" t="s">
         <v>24</v>
       </c>
       <c r="C128" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D128" t="s">
         <v>59</v>
@@ -18838,15 +18834,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B129" t="s">
         <v>24</v>
       </c>
       <c r="C129" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D129" t="s">
         <v>44</v>
@@ -18975,15 +18971,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B130" t="s">
         <v>24</v>
       </c>
       <c r="C130" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D130" t="s">
         <v>45</v>
@@ -19112,15 +19108,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B131" t="s">
         <v>24</v>
       </c>
       <c r="C131" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D131" t="s">
         <v>46</v>
@@ -19249,15 +19245,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B132" t="s">
         <v>24</v>
       </c>
       <c r="C132" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D132" t="s">
         <v>47</v>
@@ -19386,15 +19382,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B133" t="s">
         <v>24</v>
       </c>
       <c r="C133" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D133" t="s">
         <v>48</v>
@@ -19523,15 +19519,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B134" t="s">
         <v>24</v>
       </c>
       <c r="C134" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D134" t="s">
         <v>49</v>
@@ -19660,15 +19656,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B135" t="s">
         <v>24</v>
       </c>
       <c r="C135" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D135" t="s">
         <v>50</v>
@@ -19797,15 +19793,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B136" t="s">
         <v>24</v>
       </c>
       <c r="C136" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D136" t="s">
         <v>51</v>
@@ -19934,15 +19930,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B137" t="s">
         <v>24</v>
       </c>
       <c r="C137" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D137" t="s">
         <v>52</v>
@@ -20071,15 +20067,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B138" t="s">
         <v>24</v>
       </c>
       <c r="C138" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D138" t="s">
         <v>53</v>
@@ -20208,15 +20204,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B139" t="s">
         <v>24</v>
       </c>
       <c r="C139" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D139" t="s">
         <v>54</v>
@@ -20345,15 +20341,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B140" t="s">
         <v>24</v>
       </c>
       <c r="C140" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D140" t="s">
         <v>55</v>
@@ -20482,15 +20478,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B141" t="s">
         <v>24</v>
       </c>
       <c r="C141" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D141" t="s">
         <v>56</v>
@@ -20619,15 +20615,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B142" t="s">
         <v>24</v>
       </c>
       <c r="C142" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D142" t="s">
         <v>57</v>
@@ -20756,15 +20752,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B143" t="s">
         <v>24</v>
       </c>
       <c r="C143" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D143" t="s">
         <v>58</v>
@@ -20893,15 +20889,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B144" t="s">
         <v>24</v>
       </c>
       <c r="C144" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D144" t="s">
         <v>59</v>
@@ -21030,15 +21026,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B145" t="s">
         <v>24</v>
       </c>
       <c r="C145" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D145" t="s">
         <v>44</v>
@@ -21068,114 +21064,114 @@
         <v>42</v>
       </c>
       <c r="M145" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N145" t="s">
+        <v>41</v>
+      </c>
+      <c r="O145" t="s">
+        <v>43</v>
+      </c>
+      <c r="P145" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>43</v>
+      </c>
+      <c r="R145" t="s">
+        <v>41</v>
+      </c>
+      <c r="S145" t="s">
+        <v>43</v>
+      </c>
+      <c r="T145" t="s">
+        <v>41</v>
+      </c>
+      <c r="U145" t="s">
+        <v>43</v>
+      </c>
+      <c r="V145" t="s">
+        <v>41</v>
+      </c>
+      <c r="W145" t="s">
+        <v>43</v>
+      </c>
+      <c r="X145" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y145" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA145" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC145" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE145" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO145" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP145" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ145">
+        <v>0</v>
+      </c>
+      <c r="AR145">
+        <v>0</v>
+      </c>
+      <c r="AS145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>84</v>
-      </c>
-      <c r="N145" t="s">
-        <v>41</v>
-      </c>
-      <c r="O145" t="s">
-        <v>43</v>
-      </c>
-      <c r="P145" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q145" t="s">
-        <v>43</v>
-      </c>
-      <c r="R145" t="s">
-        <v>41</v>
-      </c>
-      <c r="S145" t="s">
-        <v>43</v>
-      </c>
-      <c r="T145" t="s">
-        <v>41</v>
-      </c>
-      <c r="U145" t="s">
-        <v>43</v>
-      </c>
-      <c r="V145" t="s">
-        <v>41</v>
-      </c>
-      <c r="W145" t="s">
-        <v>43</v>
-      </c>
-      <c r="X145" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y145" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA145" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC145" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE145" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AO145" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP145" t="s">
-        <v>42</v>
-      </c>
-      <c r="AQ145">
-        <v>0</v>
-      </c>
-      <c r="AR145">
-        <v>0</v>
-      </c>
-      <c r="AS145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>85</v>
       </c>
       <c r="B146" t="s">
         <v>24</v>
       </c>
       <c r="C146" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D146" t="s">
         <v>45</v>
@@ -21205,7 +21201,7 @@
         <v>42</v>
       </c>
       <c r="M146" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N146" t="s">
         <v>41</v>
@@ -21304,15 +21300,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B147" t="s">
         <v>24</v>
       </c>
       <c r="C147" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D147" t="s">
         <v>46</v>
@@ -21342,7 +21338,7 @@
         <v>42</v>
       </c>
       <c r="M147" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N147" t="s">
         <v>41</v>
@@ -21441,15 +21437,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B148" t="s">
         <v>24</v>
       </c>
       <c r="C148" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D148" t="s">
         <v>47</v>
@@ -21479,7 +21475,7 @@
         <v>42</v>
       </c>
       <c r="M148" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N148" t="s">
         <v>41</v>
@@ -21578,15 +21574,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B149" t="s">
         <v>24</v>
       </c>
       <c r="C149" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D149" t="s">
         <v>48</v>
@@ -21616,7 +21612,7 @@
         <v>42</v>
       </c>
       <c r="M149" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N149" t="s">
         <v>41</v>
@@ -21715,15 +21711,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B150" t="s">
         <v>24</v>
       </c>
       <c r="C150" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D150" t="s">
         <v>49</v>
@@ -21753,7 +21749,7 @@
         <v>42</v>
       </c>
       <c r="M150" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N150" t="s">
         <v>41</v>
@@ -21852,15 +21848,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B151" t="s">
         <v>24</v>
       </c>
       <c r="C151" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D151" t="s">
         <v>50</v>
@@ -21890,7 +21886,7 @@
         <v>42</v>
       </c>
       <c r="M151" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N151" t="s">
         <v>41</v>
@@ -21989,15 +21985,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B152" t="s">
         <v>24</v>
       </c>
       <c r="C152" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D152" t="s">
         <v>51</v>
@@ -22027,7 +22023,7 @@
         <v>42</v>
       </c>
       <c r="M152" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N152" t="s">
         <v>41</v>
@@ -22126,15 +22122,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B153" t="s">
         <v>24</v>
       </c>
       <c r="C153" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D153" t="s">
         <v>52</v>
@@ -22263,15 +22259,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B154" t="s">
         <v>24</v>
       </c>
       <c r="C154" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D154" t="s">
         <v>53</v>
@@ -22400,15 +22396,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B155" t="s">
         <v>24</v>
       </c>
       <c r="C155" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D155" t="s">
         <v>54</v>
@@ -22537,15 +22533,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B156" t="s">
         <v>24</v>
       </c>
       <c r="C156" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D156" t="s">
         <v>55</v>
@@ -22674,15 +22670,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B157" t="s">
         <v>24</v>
       </c>
       <c r="C157" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D157" t="s">
         <v>56</v>
@@ -22811,15 +22807,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B158" t="s">
         <v>24</v>
       </c>
       <c r="C158" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D158" t="s">
         <v>57</v>
@@ -22948,15 +22944,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B159" t="s">
         <v>24</v>
       </c>
       <c r="C159" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D159" t="s">
         <v>58</v>
@@ -23085,15 +23081,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B160" t="s">
         <v>24</v>
       </c>
       <c r="C160" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D160" t="s">
         <v>59</v>
@@ -23235,6 +23231,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
+    <b1b820adfd3e4a078472514c1a5cb5ff xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100260B53F379FC324F8380158707F79306" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8e72d88c5d94be5f5d36f4a7df34db">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="013edbdd-9b27-46fe-aec1-397647bd8b02" xmlns:ns3="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba157fbbfa56f81f5e8d108156af0e8f" ns2:_="" ns3:_="">
     <xsd:import namespace="013edbdd-9b27-46fe-aec1-397647bd8b02"/>
@@ -23483,28 +23500,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30452081-35FC-4E5E-B568-44E51685826A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd"/>
+    <ds:schemaRef ds:uri="013edbdd-9b27-46fe-aec1-397647bd8b02"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
-    <b1b820adfd3e4a078472514c1a5cb5ff xmlns="013edbdd-9b27-46fe-aec1-397647bd8b02" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06639B11-977A-4C9E-A3D9-282A4CA3C0CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E06B9D-EA8A-4EB0-86E2-241A21002D72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23521,23 +23536,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06639B11-977A-4C9E-A3D9-282A4CA3C0CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30452081-35FC-4E5E-B568-44E51685826A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9d7a9f5c-26b8-4c9e-9ff0-8ebffaf912dd"/>
-    <ds:schemaRef ds:uri="013edbdd-9b27-46fe-aec1-397647bd8b02"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>